<commit_message>
US-9394 [PROGRESS] PI: Changed Adjustment type to only have 2 RTs with new column. Added sub RT to Discrepancy + report and closed inventory
</commit_message>
<xml_diff>
--- a/bin/addons/stock/report/closed_physical_inventory_report.xlsx
+++ b/bin/addons/stock/report/closed_physical_inventory_report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.122.1\partage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.123.1\partage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Closed Inventory</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Inventory Date</t>
+  </si>
+  <si>
+    <t>Sub Reason Type</t>
+  </si>
+  <si>
+    <t>Encoding Error</t>
+  </si>
+  <si>
+    <t>Process Error</t>
+  </si>
+  <si>
+    <t>13 Discrepancy</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1195,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1201,12 +1213,12 @@
     <col min="9" max="9" width="15.28515625" style="14" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" customWidth="1"/>
     <col min="11" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
+    <col min="13" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1231,7 @@
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1230,7 +1242,7 @@
       <c r="I2" s="10"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>30</v>
       </c>
@@ -1250,7 +1262,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1261,7 +1273,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>31</v>
       </c>
@@ -1281,7 +1293,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1292,7 +1304,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>32</v>
       </c>
@@ -1308,7 +1320,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1319,7 +1331,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:16" s="7" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="7" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -1360,11 +1372,14 @@
         <v>16</v>
       </c>
       <c r="N9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" s="7" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" s="7" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="18" t="s">
         <v>18</v>
@@ -1387,9 +1402,10 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="25"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>1</v>
       </c>
@@ -1426,8 +1442,9 @@
         <v>24</v>
       </c>
       <c r="N11" s="24"/>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="24"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>2</v>
       </c>
@@ -1461,11 +1478,14 @@
         <v>23</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="24"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>3</v>
       </c>
@@ -1499,20 +1519,23 @@
         <v>23</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="N13" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16"/>
     </row>
     <row r="17" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>